<commit_message>
final commit for PAS-16522 automation
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_updateMSRPVersion_AZ_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_updateMSRPVersion_AZ_SS.xlsx
@@ -446,7 +446,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +552,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FB73D11-4F3D-4F04-A9D1-C0BBF1F0A20D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F23919B-2F3B-444F-B14F-E97EE1B2C3AB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>